<commit_message>
Add PPT support for the presentation
</commit_message>
<xml_diff>
--- a/Documentation/Product Backlog.xlsx
+++ b/Documentation/Product Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Montaine\Desktop\Cours HES-SO\GitHub\HEVS_S8_GIS_Camping\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4B7347-D80D-4079-860A-DD7F5F60C2DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3B164C-34D3-4181-A39D-82823F4A3C37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12384" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1028,7 +1028,7 @@
   <dimension ref="A1:XFC13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.4"/>
@@ -1093,7 +1093,9 @@
       <c r="D3" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="30"/>
+      <c r="E3" s="30">
+        <v>3</v>
+      </c>
       <c r="F3" s="30" t="s">
         <v>30</v>
       </c>
@@ -1129,7 +1131,9 @@
       <c r="D5" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="30"/>
+      <c r="E5" s="30">
+        <v>3</v>
+      </c>
       <c r="F5" s="30" t="s">
         <v>28</v>
       </c>
@@ -1147,7 +1151,9 @@
       <c r="D6" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="30"/>
+      <c r="E6" s="30">
+        <v>3</v>
+      </c>
       <c r="F6" s="30" t="s">
         <v>28</v>
       </c>
@@ -1165,7 +1171,9 @@
       <c r="D7" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="35"/>
+      <c r="E7" s="35">
+        <v>3</v>
+      </c>
       <c r="F7" s="30" t="s">
         <v>28</v>
       </c>
@@ -3227,18 +3235,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3260,6 +3268,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DCE90AB-C0FE-41BA-92CE-E86C443C4CBE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ABCF23C-177F-48BB-9CA6-65AE8594433C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -3272,12 +3288,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DCE90AB-C0FE-41BA-92CE-E86C443C4CBE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>